<commit_message>
feat: enable dense output of rodas
</commit_message>
<xml_diff>
--- a/instances/dae_test.xlsx
+++ b/instances/dae_test.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/caf4ccef320e202d/★★★科研/Solverz/Solverz/instances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_AD4DA82427541F7ACA7EB8A9580A294E6AE8DE12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6591D0CA-23BE-4D59-9488-78575375B1B5}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_AD4DA82427541F7ACA7EB8A9580A294E6AE8DE12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27B44FC6-4F82-4E0A-A452-A1DF82273E53}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="trapezoidal" sheetId="1" r:id="rId1"/>
     <sheet name="rodas" sheetId="2" r:id="rId2"/>
+    <sheet name="rodas_dense" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
     <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1993,7 +1994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39BB6F07-E782-4D02-9100-B077D94D50B3}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2083,4 +2084,1636 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F2D9002-21C6-482E-905B-187A60ED201E}">
+  <dimension ref="A1:B202"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0.958594050436958</v>
+      </c>
+      <c r="B3">
+        <v>1.03975858457155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0.93004477845703304</v>
+      </c>
+      <c r="B4">
+        <v>1.0657479327030801</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0.90991779219163904</v>
+      </c>
+      <c r="B5">
+        <v>1.0825311994923701</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0.89583375738197601</v>
+      </c>
+      <c r="B6">
+        <v>1.0938978694488299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0.885624785982987</v>
+      </c>
+      <c r="B7">
+        <v>1.1026142321130801</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0.87814149152416998</v>
+      </c>
+      <c r="B8">
+        <v>1.1086106414727701</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0.87273044760527096</v>
+      </c>
+      <c r="B9">
+        <v>1.1128240817336501</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0.86888150911943995</v>
+      </c>
+      <c r="B10">
+        <v>1.1157614615378799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0.86608453095982396</v>
+      </c>
+      <c r="B11">
+        <v>1.1179296895276001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0.86395339494812595</v>
+      </c>
+      <c r="B12">
+        <v>1.1196382645171601</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0.86237787347490702</v>
+      </c>
+      <c r="B13">
+        <v>1.12085908722264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0.86121459782890297</v>
+      </c>
+      <c r="B14">
+        <v>1.12175204613433</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0.86038297835435795</v>
+      </c>
+      <c r="B15">
+        <v>1.1223838368751999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0.85980242539551699</v>
+      </c>
+      <c r="B16">
+        <v>1.1228211550682601</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0.859392349296625</v>
+      </c>
+      <c r="B17">
+        <v>1.12313069633649</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0.85907216040192802</v>
+      </c>
+      <c r="B18">
+        <v>1.1233791563028801</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0.85880872230289496</v>
+      </c>
+      <c r="B19">
+        <v>1.12358676520002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0.85861699718350004</v>
+      </c>
+      <c r="B20">
+        <v>1.1237338992827799</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0.85846904040469996</v>
+      </c>
+      <c r="B21">
+        <v>1.1238472225613101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>0.85835897333595301</v>
+      </c>
+      <c r="B22">
+        <v>1.12393130705964</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>0.85828091734671597</v>
+      </c>
+      <c r="B23">
+        <v>1.1239907248018</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0.85822899380644602</v>
+      </c>
+      <c r="B24">
+        <v>1.12403004781178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0.85819732408460003</v>
+      </c>
+      <c r="B25">
+        <v>1.12405384811361</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0.85818002955063499</v>
+      </c>
+      <c r="B26">
+        <v>1.1240666977313001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0.85817123157400899</v>
+      </c>
+      <c r="B27">
+        <v>1.1240731686888701</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0.85816505152417799</v>
+      </c>
+      <c r="B28">
+        <v>1.12407783301034</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0.85815561077060099</v>
+      </c>
+      <c r="B29">
+        <v>1.12408526271971</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0.85813785431485301</v>
+      </c>
+      <c r="B30">
+        <v>1.1240993556568</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0.85812776395034396</v>
+      </c>
+      <c r="B31">
+        <v>1.12410707515494</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>0.85811911321470302</v>
+      </c>
+      <c r="B32">
+        <v>1.1241136922625701</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>0.85811180692389799</v>
+      </c>
+      <c r="B33">
+        <v>1.1241192799161499</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0.85810574989390198</v>
+      </c>
+      <c r="B34">
+        <v>1.1241239110521599</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>0.858100846940683</v>
+      </c>
+      <c r="B35">
+        <v>1.1241276586070399</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>0.85809700288021196</v>
+      </c>
+      <c r="B36">
+        <v>1.12413059551728</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>0.85809412252846096</v>
+      </c>
+      <c r="B37">
+        <v>1.12413279471934</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>0.85809211070139702</v>
+      </c>
+      <c r="B38">
+        <v>1.1241343291496799</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>0.85809087221499403</v>
+      </c>
+      <c r="B39">
+        <v>1.1241352717447699</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>0.858090311885219</v>
+      </c>
+      <c r="B40">
+        <v>1.1241356954410699</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>0.85809033452804495</v>
+      </c>
+      <c r="B41">
+        <v>1.12413567317504</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>0.85809084495943999</v>
+      </c>
+      <c r="B42">
+        <v>1.1241352778831699</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>0.85809174799537602</v>
+      </c>
+      <c r="B43">
+        <v>1.1241345825019</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>0.85809294845182305</v>
+      </c>
+      <c r="B44">
+        <v>1.1241336599677101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>0.85809435114474997</v>
+      </c>
+      <c r="B45">
+        <v>1.1241325832170601</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>0.85809586089013001</v>
+      </c>
+      <c r="B46">
+        <v>1.1241314251864101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>0.85809738250392997</v>
+      </c>
+      <c r="B47">
+        <v>1.1241302588122399</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>0.85809882080212296</v>
+      </c>
+      <c r="B48">
+        <v>1.1241291570310099</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>0.85810008060067799</v>
+      </c>
+      <c r="B49">
+        <v>1.12412819277918</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>0.85810106671556596</v>
+      </c>
+      <c r="B50">
+        <v>1.1241274389932101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>0.85810168396275599</v>
+      </c>
+      <c r="B51">
+        <v>1.12412696860959</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>0.85810183715821997</v>
+      </c>
+      <c r="B52">
+        <v>1.12412685456476</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>0.85810143111792703</v>
+      </c>
+      <c r="B53">
+        <v>1.1241271697952</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>0.85810037065784905</v>
+      </c>
+      <c r="B54">
+        <v>1.12412798723736</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>0.85809871062837595</v>
+      </c>
+      <c r="B55">
+        <v>1.12412926409699</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>0.85809808452567204</v>
+      </c>
+      <c r="B56">
+        <v>1.1241297420704199</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>0.85809749595407103</v>
+      </c>
+      <c r="B57">
+        <v>1.12413019139181</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>0.85809694400560299</v>
+      </c>
+      <c r="B58">
+        <v>1.12413061275434</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>0.858096427772296</v>
+      </c>
+      <c r="B59">
+        <v>1.1241310068511601</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>0.85809594634617803</v>
+      </c>
+      <c r="B60">
+        <v>1.12413137437546</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>0.85809549881927905</v>
+      </c>
+      <c r="B61">
+        <v>1.1241317160204101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>0.85809508428362702</v>
+      </c>
+      <c r="B62">
+        <v>1.1241320324791599</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>0.85809470183125003</v>
+      </c>
+      <c r="B63">
+        <v>1.12413232444491</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>0.85809435055417804</v>
+      </c>
+      <c r="B64">
+        <v>1.1241325926108101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>0.85809402954443903</v>
+      </c>
+      <c r="B65">
+        <v>1.1241328376700299</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>0.85809373789406096</v>
+      </c>
+      <c r="B66">
+        <v>1.12413306031576</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>0.85809347469507302</v>
+      </c>
+      <c r="B67">
+        <v>1.1241332612411501</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>0.85809323903950396</v>
+      </c>
+      <c r="B68">
+        <v>1.12413344113938</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>0.85809303001938297</v>
+      </c>
+      <c r="B69">
+        <v>1.12413360070361</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>0.85809284672673802</v>
+      </c>
+      <c r="B70">
+        <v>1.12413374062703</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>0.85809268825359797</v>
+      </c>
+      <c r="B71">
+        <v>1.1241338616027901</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>0.858092553691991</v>
+      </c>
+      <c r="B72">
+        <v>1.12413396432408</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>0.85809244213394598</v>
+      </c>
+      <c r="B73">
+        <v>1.1241340494840599</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>0.85809235267149297</v>
+      </c>
+      <c r="B74">
+        <v>1.1241341177758899</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>0.85809228439665797</v>
+      </c>
+      <c r="B75">
+        <v>1.12413416989276</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>0.85809223640147203</v>
+      </c>
+      <c r="B76">
+        <v>1.1241342065278299</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>0.85809220777796302</v>
+      </c>
+      <c r="B77">
+        <v>1.1241342283742799</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>0.85809219761815902</v>
+      </c>
+      <c r="B78">
+        <v>1.12413423612527</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>0.858092205014089</v>
+      </c>
+      <c r="B79">
+        <v>1.1241342304739701</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>0.85809222905778204</v>
+      </c>
+      <c r="B80">
+        <v>1.12413421211356</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>0.85809226884126699</v>
+      </c>
+      <c r="B81">
+        <v>1.1241341817371999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>0.85809232345657105</v>
+      </c>
+      <c r="B82">
+        <v>1.12413414003807</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>0.85809239199572396</v>
+      </c>
+      <c r="B83">
+        <v>1.12413408770933</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>0.85809247355075502</v>
+      </c>
+      <c r="B84">
+        <v>1.1241340254441601</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>0.85809256721369098</v>
+      </c>
+      <c r="B85">
+        <v>1.12413395393573</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>0.85809267207656303</v>
+      </c>
+      <c r="B86">
+        <v>1.12413387387721</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>0.85809278723139704</v>
+      </c>
+      <c r="B87">
+        <v>1.1241337859617599</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>0.85809291177022395</v>
+      </c>
+      <c r="B88">
+        <v>1.1241336908825701</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>0.85809304478507098</v>
+      </c>
+      <c r="B89">
+        <v>1.12413358933279</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>0.85809318536796697</v>
+      </c>
+      <c r="B90">
+        <v>1.1241334820055999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>0.85809333261094201</v>
+      </c>
+      <c r="B91">
+        <v>1.12413336959418</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>0.85809348560602305</v>
+      </c>
+      <c r="B92">
+        <v>1.1241332527916801</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>0.85809364344523997</v>
+      </c>
+      <c r="B93">
+        <v>1.12413313229129</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>0.85809380522061995</v>
+      </c>
+      <c r="B94">
+        <v>1.1241330087861701</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>0.85809397002419296</v>
+      </c>
+      <c r="B95">
+        <v>1.1241328829694901</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>0.85809413694798697</v>
+      </c>
+      <c r="B96">
+        <v>1.12413275553443</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>0.85809430508403095</v>
+      </c>
+      <c r="B97">
+        <v>1.1241326271741501</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>0.85809447352435397</v>
+      </c>
+      <c r="B98">
+        <v>1.12413249858183</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>0.85809464136098401</v>
+      </c>
+      <c r="B99">
+        <v>1.1241323704506301</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>0.85809480768594903</v>
+      </c>
+      <c r="B100">
+        <v>1.12413224347372</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>0.85809497159128001</v>
+      </c>
+      <c r="B101">
+        <v>1.1241321183442801</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>0.85809513216900302</v>
+      </c>
+      <c r="B102">
+        <v>1.1241319957554801</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>0.85809528851114802</v>
+      </c>
+      <c r="B103">
+        <v>1.1241318764004899</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>0.858095439709744</v>
+      </c>
+      <c r="B104">
+        <v>1.1241317609724699</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>0.85809558485681903</v>
+      </c>
+      <c r="B105">
+        <v>1.1241316501645999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>0.85809572304440196</v>
+      </c>
+      <c r="B106">
+        <v>1.1241315446700499</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>0.85809585336452099</v>
+      </c>
+      <c r="B107">
+        <v>1.1241314451819899</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>0.85809597490920497</v>
+      </c>
+      <c r="B108">
+        <v>1.1241313523935901</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>0.85809608677048299</v>
+      </c>
+      <c r="B109">
+        <v>1.1241312669980299</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>0.85809618804038401</v>
+      </c>
+      <c r="B110">
+        <v>1.12413118968846</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>0.858096277810935</v>
+      </c>
+      <c r="B111">
+        <v>1.12413112115806</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>0.85809635517416605</v>
+      </c>
+      <c r="B112">
+        <v>1.12413106210001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>0.858096419222106</v>
+      </c>
+      <c r="B113">
+        <v>1.12413101320747</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>0.85809646904678305</v>
+      </c>
+      <c r="B114">
+        <v>1.1241309751736099</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>0.85809650374022495</v>
+      </c>
+      <c r="B115">
+        <v>1.12413094869161</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>0.85809652239446199</v>
+      </c>
+      <c r="B116">
+        <v>1.12413093445463</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>0.85809652410152204</v>
+      </c>
+      <c r="B117">
+        <v>1.12413093315584</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>0.85809650795343295</v>
+      </c>
+      <c r="B118">
+        <v>1.1241309454884301</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>0.85809647304222503</v>
+      </c>
+      <c r="B119">
+        <v>1.1241309721455399</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>0.85809641845992601</v>
+      </c>
+      <c r="B120">
+        <v>1.12413101382037</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>0.85809634329856499</v>
+      </c>
+      <c r="B121">
+        <v>1.1241310712060699</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>0.85809624665016904</v>
+      </c>
+      <c r="B122">
+        <v>1.12413114499582</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>0.85809612760676901</v>
+      </c>
+      <c r="B123">
+        <v>1.12413123588279</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>0.85809598526039199</v>
+      </c>
+      <c r="B124">
+        <v>1.12413134456015</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>0.85809581870306795</v>
+      </c>
+      <c r="B125">
+        <v>1.12413147172106</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>0.85809562702682396</v>
+      </c>
+      <c r="B126">
+        <v>1.12413161805871</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>0.85809540932368999</v>
+      </c>
+      <c r="B127">
+        <v>1.1241317842662599</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>0.85809516468569502</v>
+      </c>
+      <c r="B128">
+        <v>1.12413197103687</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>0.85809498886511204</v>
+      </c>
+      <c r="B129">
+        <v>1.1241321052618301</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>0.85809489077267198</v>
+      </c>
+      <c r="B130">
+        <v>1.12413218014019</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>0.85809479865883098</v>
+      </c>
+      <c r="B131">
+        <v>1.1241322504548099</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>0.85809471237735502</v>
+      </c>
+      <c r="B132">
+        <v>1.12413231631732</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>0.85809463178201195</v>
+      </c>
+      <c r="B133">
+        <v>1.1241323778393399</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>0.85809455672656898</v>
+      </c>
+      <c r="B134">
+        <v>1.1241324351325099</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>0.85809448706479297</v>
+      </c>
+      <c r="B135">
+        <v>1.12413248830844</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>0.85809442265045199</v>
+      </c>
+      <c r="B136">
+        <v>1.1241325374787601</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>0.85809436333731404</v>
+      </c>
+      <c r="B137">
+        <v>1.1241325827551001</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>0.85809430897914396</v>
+      </c>
+      <c r="B138">
+        <v>1.1241326242490799</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>0.85809425942971096</v>
+      </c>
+      <c r="B139">
+        <v>1.12413266207234</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>0.85809421454278201</v>
+      </c>
+      <c r="B140">
+        <v>1.1241326963364899</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>0.85809417417212397</v>
+      </c>
+      <c r="B141">
+        <v>1.12413272715317</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>0.85809413817150504</v>
+      </c>
+      <c r="B142">
+        <v>1.1241327546340001</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>0.85809410639469197</v>
+      </c>
+      <c r="B143">
+        <v>1.1241327788905999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>0.85809407869545196</v>
+      </c>
+      <c r="B144">
+        <v>1.12413280003461</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>0.85809405492755197</v>
+      </c>
+      <c r="B145">
+        <v>1.12413281817764</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>0.85809403494476</v>
+      </c>
+      <c r="B146">
+        <v>1.1241328334313301</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>0.858094018600843</v>
+      </c>
+      <c r="B147">
+        <v>1.1241328459072999</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>0.85809400574956796</v>
+      </c>
+      <c r="B148">
+        <v>1.1241328557171799</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>0.85809399624470295</v>
+      </c>
+      <c r="B149">
+        <v>1.12413286297259</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>0.85809398994001496</v>
+      </c>
+      <c r="B150">
+        <v>1.1241328677851601</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>0.85809398668927195</v>
+      </c>
+      <c r="B151">
+        <v>1.1241328702665201</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>0.85809398634623901</v>
+      </c>
+      <c r="B152">
+        <v>1.12413287052829</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>0.85809398876468601</v>
+      </c>
+      <c r="B153">
+        <v>1.1241328686820899</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>0.85809399379837903</v>
+      </c>
+      <c r="B154">
+        <v>1.1241328648395701</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>0.85809400130108604</v>
+      </c>
+      <c r="B155">
+        <v>1.1241328591123301</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>0.85809401112657302</v>
+      </c>
+      <c r="B156">
+        <v>1.1241328516120099</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>0.85809402312860805</v>
+      </c>
+      <c r="B157">
+        <v>1.1241328424502299</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>0.858094037160959</v>
+      </c>
+      <c r="B158">
+        <v>1.1241328317386301</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>0.85809405307739195</v>
+      </c>
+      <c r="B159">
+        <v>1.1241328195888101</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>0.85809407073167598</v>
+      </c>
+      <c r="B160">
+        <v>1.1241328061124201</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>0.85809408997757697</v>
+      </c>
+      <c r="B161">
+        <v>1.1241327914210799</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>0.85809411066886199</v>
+      </c>
+      <c r="B162">
+        <v>1.1241327756264199</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>0.85809413265930001</v>
+      </c>
+      <c r="B163">
+        <v>1.12413275884005</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>0.85809415580265602</v>
+      </c>
+      <c r="B164">
+        <v>1.12413274117361</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>0.85809417995269899</v>
+      </c>
+      <c r="B165">
+        <v>1.1241327227387301</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>0.85809420496319599</v>
+      </c>
+      <c r="B166">
+        <v>1.1241327036470199</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>0.85809423068791402</v>
+      </c>
+      <c r="B167">
+        <v>1.12413268401012</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>0.85809425698062103</v>
+      </c>
+      <c r="B168">
+        <v>1.1241326639396501</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>0.858094283695083</v>
+      </c>
+      <c r="B169">
+        <v>1.1241326435472401</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>0.85809431068506903</v>
+      </c>
+      <c r="B170">
+        <v>1.1241326229445201</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>0.85809433780434397</v>
+      </c>
+      <c r="B171">
+        <v>1.1241326022431</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>0.85809436490667801</v>
+      </c>
+      <c r="B172">
+        <v>1.1241325815546299</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>0.85809439184583602</v>
+      </c>
+      <c r="B173">
+        <v>1.12413256099071</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <v>0.85809441847558698</v>
+      </c>
+      <c r="B174">
+        <v>1.1241325406629901</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>0.85809444464969697</v>
+      </c>
+      <c r="B175">
+        <v>1.1241325206830799</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176">
+        <v>0.85809447022193397</v>
+      </c>
+      <c r="B176">
+        <v>1.12413250116261</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177">
+        <v>0.85809449504606605</v>
+      </c>
+      <c r="B177">
+        <v>1.1241324822132099</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>0.85809451897585798</v>
+      </c>
+      <c r="B178">
+        <v>1.1241324639465</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179">
+        <v>0.85809454186508005</v>
+      </c>
+      <c r="B179">
+        <v>1.12413244647412</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A180">
+        <v>0.85809456356749803</v>
+      </c>
+      <c r="B180">
+        <v>1.12413242990768</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A181">
+        <v>0.85809458393687899</v>
+      </c>
+      <c r="B181">
+        <v>1.1241324143588101</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A182">
+        <v>0.85809460282699102</v>
+      </c>
+      <c r="B182">
+        <v>1.1241323999391499</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A183">
+        <v>0.85809462009160098</v>
+      </c>
+      <c r="B183">
+        <v>1.1241323867602999</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A184">
+        <v>0.85809463558447596</v>
+      </c>
+      <c r="B184">
+        <v>1.1241323749339101</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A185">
+        <v>0.85809464915938405</v>
+      </c>
+      <c r="B185">
+        <v>1.1241323645715999</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A186">
+        <v>0.85809466067009099</v>
+      </c>
+      <c r="B186">
+        <v>1.124132355785</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A187">
+        <v>0.85809466997036599</v>
+      </c>
+      <c r="B187">
+        <v>1.12413234868572</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A188">
+        <v>0.85809467691397601</v>
+      </c>
+      <c r="B188">
+        <v>1.1241323433854</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A189">
+        <v>0.85809468135468703</v>
+      </c>
+      <c r="B189">
+        <v>1.12413233999566</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A190">
+        <v>0.85809468314626802</v>
+      </c>
+      <c r="B190">
+        <v>1.1241323386281299</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A191">
+        <v>0.85809468214248497</v>
+      </c>
+      <c r="B191">
+        <v>1.12413233939444</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A192">
+        <v>0.85809467819710605</v>
+      </c>
+      <c r="B192">
+        <v>1.12413234240621</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A193">
+        <v>0.85809467116389704</v>
+      </c>
+      <c r="B193">
+        <v>1.12413234777506</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A194">
+        <v>0.858094660896628</v>
+      </c>
+      <c r="B194">
+        <v>1.1241323556126299</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A195">
+        <v>0.85809464724906304</v>
+      </c>
+      <c r="B195">
+        <v>1.12413236603054</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A196">
+        <v>0.858094630074972</v>
+      </c>
+      <c r="B196">
+        <v>1.1241323791404201</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A197">
+        <v>0.85809460922812097</v>
+      </c>
+      <c r="B197">
+        <v>1.12413239505389</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A198">
+        <v>0.85809458456227805</v>
+      </c>
+      <c r="B198">
+        <v>1.1241324138825799</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A199">
+        <v>0.85809455593120998</v>
+      </c>
+      <c r="B199">
+        <v>1.1241324357381099</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A200">
+        <v>0.85809452318868296</v>
+      </c>
+      <c r="B200">
+        <v>1.1241324607321199</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A201">
+        <v>0.85809448618846695</v>
+      </c>
+      <c r="B201">
+        <v>1.1241324889762201</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A202">
+        <v>0.85809444478432695</v>
+      </c>
+      <c r="B202">
+        <v>1.12413252058205</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>